<commit_message>
Revision of Chapter 7-9
</commit_message>
<xml_diff>
--- a/extras/ChartsClinicalValidity.xlsx
+++ b/extras/ChartsClinicalValidity.xlsx
@@ -1055,8 +1055,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0e002fabf17cb2440d8e9a473d3a41c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4cec627508c1f1ba247db94416ea198" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="a9cab35011a557c1232e9e1918db7064">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36c473bbc383ceb924bb8d2cdd9a2de6" ns2:_="" ns3:_="">
     <xsd:import namespace="180f08d8-883b-45c0-bb81-5ddbcba5023b"/>
     <xsd:import namespace="e3b36e9c-ff3c-4531-9d5c-178a6758d490"/>
     <xsd:element name="properties">
@@ -1105,7 +1105,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="画像タグ" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1159,8 +1159,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="コンテンツ タイプ"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="タイトル"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1270,7 +1270,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD48CF6-4EF7-48CB-A010-3494A0B123E2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{670A6183-C468-4C6D-AD57-6B622B4ED095}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Revert the changes in Figures.
</commit_message>
<xml_diff>
--- a/extras/ChartsClinicalValidity.xlsx
+++ b/extras/ChartsClinicalValidity.xlsx
@@ -1055,8 +1055,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="a9cab35011a557c1232e9e1918db7064">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36c473bbc383ceb924bb8d2cdd9a2de6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0e002fabf17cb2440d8e9a473d3a41c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4cec627508c1f1ba247db94416ea198" ns2:_="" ns3:_="">
     <xsd:import namespace="180f08d8-883b-45c0-bb81-5ddbcba5023b"/>
     <xsd:import namespace="e3b36e9c-ff3c-4531-9d5c-178a6758d490"/>
     <xsd:element name="properties">
@@ -1105,7 +1105,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="画像タグ" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1159,8 +1159,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="コンテンツ タイプ"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="タイトル"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1270,7 +1270,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FD25FF8-BEB1-4182-BAAD-E5D8D24DA03B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A06E3DD-4DB2-495B-8E8C-D01EB0E4922F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Attempt to fix merge issues.
</commit_message>
<xml_diff>
--- a/extras/ChartsClinicalValidity.xlsx
+++ b/extras/ChartsClinicalValidity.xlsx
@@ -1055,8 +1055,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="a9cab35011a557c1232e9e1918db7064">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36c473bbc383ceb924bb8d2cdd9a2de6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6AD93ACCF9B89429D5F814A1B934813" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0e002fabf17cb2440d8e9a473d3a41c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f08d8-883b-45c0-bb81-5ddbcba5023b" xmlns:ns3="e3b36e9c-ff3c-4531-9d5c-178a6758d490" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4cec627508c1f1ba247db94416ea198" ns2:_="" ns3:_="">
     <xsd:import namespace="180f08d8-883b-45c0-bb81-5ddbcba5023b"/>
     <xsd:import namespace="e3b36e9c-ff3c-4531-9d5c-178a6758d490"/>
     <xsd:element name="properties">
@@ -1105,7 +1105,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="画像タグ" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4989c4a-421d-4ebb-87fd-c2bbc6e780fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1159,8 +1159,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="コンテンツ タイプ"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="タイトル"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1270,7 +1270,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25771E2D-8D12-4709-8031-9244DF208EB6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F0FD158-B063-49EE-ABD2-978475912075}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>